<commit_message>
Added LegendSetup and other fixes
</commit_message>
<xml_diff>
--- a/ClueRooms.xlsx
+++ b/ClueRooms.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306work\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Software Engineering\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="8055"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ClueRooms" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -447,7 +447,7 @@
   <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>